<commit_message>
Add the index column
</commit_message>
<xml_diff>
--- a/ACP Data.xlsx
+++ b/ACP Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b04d825435d036ce/Documents/ACP Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C43CF04A-5952-4945-8F94-7F225CFD74C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C43CF04A-5952-4945-8F94-7F225CFD74C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEEB2A5B-A625-4442-89BC-8D241BC03E07}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{84048566-F36F-4C7D-90A8-BFA1C22116A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Pain ordinaire (PAO)</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Inactifs (INAC)</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
@@ -457,9 +460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457539DB-75BA-418B-B5B0-27472BD1DED2}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -475,6 +476,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>

</xml_diff>